<commit_message>
Fixed barriers and naming
</commit_message>
<xml_diff>
--- a/Output/CorrelationsAll.xlsx
+++ b/Output/CorrelationsAll.xlsx
@@ -507,7 +507,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.03</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.03</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>0.08***</t>
+          <t>0.07**</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -783,12 +783,12 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>-0.01</t>
+          <t>-0.05*</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.14***</t>
+          <t>0.15***</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -875,12 +875,12 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>-0.05</t>
+          <t>-0.06*</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.08***</t>
+          <t>0.09***</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -967,7 +967,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>-0.11***</t>
+          <t>-0.15***</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1059,12 +1059,12 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.05</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>-0.03</t>
+          <t>-0.04</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>-0.05*</t>
+          <t>-0.06*</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>0.03</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1335,12 +1335,12 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.03</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.06**</t>
+          <t>0.07**</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1377,37 +1377,37 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>0.03</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>-0.02</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.13</t>
+          <t>0.04</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-0.05</t>
+          <t>-0.20</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>0.09</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>-0.03</t>
+          <t>-0.16</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.23</t>
+          <t>0.20</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1417,47 +1417,47 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>[0.08]</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>-0.44***</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>-0.01</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0.07**</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>0.06**</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
           <t>-0.04</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>[0.09]</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>-0.46***</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>-0.00</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>0.11***</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>0.06*</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>-0.03</t>
         </is>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>-0.10</t>
+          <t>-0.08</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1489,17 +1489,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.05</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>0.02</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>-0.06</t>
+          <t>-0.05</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1519,12 +1519,12 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>-0.02</t>
+          <t>-0.13</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>[0.28]</t>
+          <t>[0.29]</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1611,12 +1611,12 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>-0.14</t>
+          <t>-0.26</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>0.34*</t>
+          <t>0.36*</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1703,12 +1703,12 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>-0.01</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1795,12 +1795,12 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>-0.01</t>
+          <t>-0.10</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>0.22</t>
+          <t>0.23</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>-0.03</t>
+          <t>-0.02</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1979,12 +1979,12 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.12</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>-0.27</t>
+          <t>-0.24</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">

</xml_diff>